<commit_message>
add vlan pools config
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\ubuntu-22.04\home\mark\terraform\intro_with_aci_non_tfe_version\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\ubuntu-22.04\home\mark\terraform\aci_config_terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD393E68-C097-4932-8275-11350CE2D5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1251FB-C6AA-4064-9B36-A230ADF4B99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57915" yWindow="1005" windowWidth="28095" windowHeight="14355" tabRatio="323" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58500" yWindow="1125" windowWidth="27825" windowHeight="14505" tabRatio="323" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TENANT" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,15 @@
     <sheet name="SUBNET" sheetId="3" r:id="rId4"/>
     <sheet name="APP_PROFILE" sheetId="4" r:id="rId5"/>
     <sheet name="EPG" sheetId="5" r:id="rId6"/>
+    <sheet name="VLAN_POOL" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>type</t>
   </si>
@@ -112,6 +114,24 @@
   </si>
   <si>
     <t>subnet_description</t>
+  </si>
+  <si>
+    <t>vlan_pool</t>
+  </si>
+  <si>
+    <t>vlan_pool_name</t>
+  </si>
+  <si>
+    <t>range_from</t>
+  </si>
+  <si>
+    <t>range_to</t>
+  </si>
+  <si>
+    <t>mark_pool</t>
+  </si>
+  <si>
+    <t>allocation_mode</t>
   </si>
 </sst>
 </file>
@@ -578,9 +598,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1016,7 +1039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -1150,7 +1173,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1191,4 +1214,252 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B67D955-82DD-4325-AFFB-135E2F3A7F6E}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.296875" customWidth="1"/>
+    <col min="2" max="2" width="21.796875" customWidth="1"/>
+    <col min="3" max="3" width="30.3984375" customWidth="1"/>
+    <col min="4" max="4" width="20.09765625" customWidth="1"/>
+    <col min="5" max="5" width="28.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1024</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1034</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECFB55F-691D-41CF-90DB-1F34F9822B23}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added phys domain resource
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\ubuntu-22.04\home\mark\terraform\aci_config_terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E962429F-7038-4056-B15F-89D3CF7C8224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD7BE0A-3769-4243-AEF4-313A2D223004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58530" yWindow="675" windowWidth="27825" windowHeight="14505" tabRatio="323" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58410" yWindow="1095" windowWidth="27825" windowHeight="14505" tabRatio="463" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TENANT" sheetId="1" r:id="rId1"/>
     <sheet name="VRF" sheetId="6" r:id="rId2"/>
-    <sheet name="BD" sheetId="2" r:id="rId3"/>
-    <sheet name="SUBNET" sheetId="3" r:id="rId4"/>
-    <sheet name="APP_PROFILE" sheetId="4" r:id="rId5"/>
+    <sheet name="APP_PROFILE" sheetId="4" r:id="rId3"/>
+    <sheet name="BD" sheetId="2" r:id="rId4"/>
+    <sheet name="SUBNET" sheetId="3" r:id="rId5"/>
     <sheet name="EPG" sheetId="5" r:id="rId6"/>
     <sheet name="VLAN_POOL" sheetId="8" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId8"/>
+    <sheet name="PHYSICAL_DOMAIN" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>type</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>vlan-1034</t>
+  </si>
+  <si>
+    <t>physical_domain</t>
+  </si>
+  <si>
+    <t>physical_domain_name</t>
+  </si>
+  <si>
+    <t>markacidomain</t>
   </si>
 </sst>
 </file>
@@ -1045,6 +1054,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.09765625" customWidth="1"/>
+    <col min="2" max="2" width="27.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1086,7 +1130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1135,41 +1179,6 @@
       </c>
       <c r="E2" t="s">
         <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.09765625" customWidth="1"/>
-    <col min="2" max="2" width="27.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1229,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B67D955-82DD-4325-AFFB-135E2F3A7F6E}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1465,12 +1474,46 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECFB55F-691D-41CF-90DB-1F34F9822B23}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.296875" customWidth="1"/>
+    <col min="2" max="2" width="23.69921875" customWidth="1"/>
+    <col min="3" max="3" width="18.796875" customWidth="1"/>
+    <col min="4" max="4" width="20.69921875" customWidth="1"/>
+    <col min="5" max="5" width="24.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add new bd and epg
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\ubuntu-22.04\home\mark\terraform\aci_config_terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B591E192-E3BD-404F-A37D-BBEC49A6F9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D80638E-BF50-44DD-BA39-DCBCBF60E9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58410" yWindow="1095" windowWidth="27825" windowHeight="14505" tabRatio="463" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58410" yWindow="1095" windowWidth="27825" windowHeight="14505" tabRatio="463" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TENANT" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>type</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>mode</t>
+  </si>
+  <si>
+    <t>mark_second_bd_for_subnet</t>
+  </si>
+  <si>
+    <t>This other  bridge domain is created by the Terraform ACI provider1</t>
+  </si>
+  <si>
+    <t>mark_second_epg</t>
   </si>
 </sst>
 </file>
@@ -1093,16 +1102,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.796875" customWidth="1"/>
-    <col min="3" max="3" width="52.69921875" customWidth="1"/>
+    <col min="3" max="3" width="56.09765625" customWidth="1"/>
     <col min="4" max="4" width="27.8984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1126,6 +1135,17 @@
       </c>
       <c r="C2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1191,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1229,6 +1249,20 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1479,7 +1513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECFB55F-691D-41CF-90DB-1F34F9822B23}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add sixth bd and epg
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\ubuntu-22.04\home\mark\terraform\aci_config_terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6082C1-14C2-4998-9235-B387920672BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940620AB-8361-4818-A91B-603577F7C88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29040" yWindow="120" windowWidth="27840" windowHeight="15270" tabRatio="737" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29325" yWindow="345" windowWidth="27840" windowHeight="15270" tabRatio="737" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TENANT" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="126">
   <si>
     <t>type</t>
   </si>
@@ -401,6 +401,15 @@
   </si>
   <si>
     <t>mark_fifth_epg</t>
+  </si>
+  <si>
+    <t>mark_sixth_bd_for_subnet</t>
+  </si>
+  <si>
+    <t>This 6th  bridge domain is created by the Terraform ACI provider</t>
+  </si>
+  <si>
+    <t>mark_sixth_epg</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1240,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1275,7 +1284,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1520,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B412DCD1-4318-455B-9FD4-CC49F307448F}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1716,7 +1725,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1782,10 +1791,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1861,6 +1870,17 @@
         <v>118</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1868,10 +1888,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1965,6 +1985,20 @@
         <v>49</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1975,7 +2009,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added vrfs and tenants
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\ubuntu-22.04\home\mark\terraform\aci_config_terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F235968B-C20F-480E-9988-7965B230A0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DCF5AF-9B56-48A8-92B4-1622810AA651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29130" yWindow="105" windowWidth="28140" windowHeight="14925" tabRatio="737" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58425" yWindow="450" windowWidth="27495" windowHeight="14925" tabRatio="737" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TENANT" sheetId="1" r:id="rId1"/>
     <sheet name="VRF" sheetId="6" r:id="rId2"/>
-    <sheet name="BD" sheetId="2" r:id="rId3"/>
-    <sheet name="SUBNET" sheetId="3" r:id="rId4"/>
-    <sheet name="APP_PROFILE" sheetId="4" r:id="rId5"/>
-    <sheet name="EPG" sheetId="5" r:id="rId6"/>
+    <sheet name="APP_PROFILE" sheetId="4" r:id="rId3"/>
+    <sheet name="BD" sheetId="2" r:id="rId4"/>
+    <sheet name="EPG" sheetId="5" r:id="rId5"/>
+    <sheet name="SUBNET" sheetId="3" r:id="rId6"/>
     <sheet name="VLAN_POOL" sheetId="8" r:id="rId7"/>
     <sheet name="PHYSICAL_DOMAIN" sheetId="7" r:id="rId8"/>
     <sheet name="AAEP" sheetId="9" r:id="rId9"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="144">
   <si>
     <t>type</t>
   </si>
@@ -67,9 +67,6 @@
     <t>tenant</t>
   </si>
   <si>
-    <t>marks_first_tenant</t>
-  </si>
-  <si>
     <t>This bridge domain is created by the Terraform ACI provider1</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>app_profile</t>
   </si>
   <si>
-    <t>marks_vrf</t>
-  </si>
-  <si>
     <t>vrf</t>
   </si>
   <si>
@@ -419,6 +413,57 @@
   </si>
   <si>
     <t>mark_seventh_epg</t>
+  </si>
+  <si>
+    <t>vrf_tenant</t>
+  </si>
+  <si>
+    <t>bd_associated_tenant</t>
+  </si>
+  <si>
+    <t>bd_associated_vrf</t>
+  </si>
+  <si>
+    <t>subnet_associated_tenant</t>
+  </si>
+  <si>
+    <t>app_profile_associated_tenant</t>
+  </si>
+  <si>
+    <t>epg_associated_tenant</t>
+  </si>
+  <si>
+    <t>marks_network_centric</t>
+  </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>marks_vrf_lan</t>
+  </si>
+  <si>
+    <t>marks_vrf_dmz</t>
+  </si>
+  <si>
+    <t>mark_1st_dmz_bd_for_subnet</t>
+  </si>
+  <si>
+    <t>mark_2nd_dmz_bd_for_subnet</t>
+  </si>
+  <si>
+    <t>dmz1</t>
+  </si>
+  <si>
+    <t>mark_1st_dmz__epg</t>
+  </si>
+  <si>
+    <t>mark_2nd_dmz_epg</t>
+  </si>
+  <si>
+    <t>prod_dmz_app_profile</t>
+  </si>
+  <si>
+    <t>dmz2_</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1291,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1277,10 +1322,18 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1310,160 +1363,160 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
         <v>62</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E5">
         <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E6">
         <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E7">
         <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1492,41 +1545,41 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>86</v>
-      </c>
-      <c r="C2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
         <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1555,30 +1608,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1587,7 +1640,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1617,33 +1670,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1651,21 +1704,21 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1673,21 +1726,21 @@
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C8" s="2">
         <v>55</v>
@@ -1701,21 +1754,21 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" s="2">
         <v>101</v>
@@ -1731,31 +1784,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.796875" customWidth="1"/>
+    <col min="3" max="3" width="32.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1764,11 +1835,64 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.09765625" customWidth="1"/>
+    <col min="2" max="2" width="27.59765625" customWidth="1"/>
+    <col min="3" max="3" width="36.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1776,9 +1900,10 @@
     <col min="2" max="2" width="26.796875" customWidth="1"/>
     <col min="3" max="3" width="70.09765625" customWidth="1"/>
     <col min="4" max="4" width="27.8984375" customWidth="1"/>
+    <col min="5" max="5" width="32.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1788,82 +1913,164 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>126</v>
-      </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E10" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1871,12 +2078,203 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.296875" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="40.59765625" customWidth="1"/>
+    <col min="5" max="5" width="52.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1886,207 +2284,47 @@
     <col min="3" max="3" width="31.59765625" customWidth="1"/>
     <col min="4" max="4" width="21.09765625" customWidth="1"/>
     <col min="5" max="5" width="38.796875" customWidth="1"/>
+    <col min="6" max="6" width="35.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.09765625" customWidth="1"/>
-    <col min="2" max="2" width="27.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.296875" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="40.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
+      <c r="F2" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2116,33 +2354,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2354,28 +2592,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
       <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2402,21 +2640,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add long bd name
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\ubuntu-22.04\home\mark\terraform\aci_config_terraform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DCF5AF-9B56-48A8-92B4-1622810AA651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49838C8-943E-4B49-B4C8-4A1BFB7029AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58425" yWindow="450" windowWidth="27495" windowHeight="14925" tabRatio="737" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60585" yWindow="1125" windowWidth="22815" windowHeight="11700" tabRatio="737" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TENANT" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="146">
   <si>
     <t>type</t>
   </si>
@@ -464,6 +464,12 @@
   </si>
   <si>
     <t>dmz2_</t>
+  </si>
+  <si>
+    <t>bd_vlan996_10.255.60.0_255.255.255.224_oob_mgt_internet</t>
+  </si>
+  <si>
+    <t>epg_vlan996_10.255.60.0_255.255.255.224_oob_mgt_internet</t>
   </si>
 </sst>
 </file>
@@ -1889,15 +1895,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D11" sqref="D11:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.796875" customWidth="1"/>
+    <col min="2" max="2" width="51.8984375" customWidth="1"/>
     <col min="3" max="3" width="70.09765625" customWidth="1"/>
     <col min="4" max="4" width="27.8984375" customWidth="1"/>
     <col min="5" max="5" width="32.59765625" customWidth="1"/>
@@ -2073,6 +2079,20 @@
         <v>136</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2080,16 +2100,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.296875" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="2" max="2" width="54.8984375" customWidth="1"/>
+    <col min="3" max="3" width="55.59765625" customWidth="1"/>
     <col min="4" max="4" width="40.59765625" customWidth="1"/>
     <col min="5" max="5" width="52.59765625" customWidth="1"/>
   </cols>
@@ -2261,6 +2281,23 @@
         <v>142</v>
       </c>
       <c r="E10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2336,7 +2373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B67D955-82DD-4325-AFFB-135E2F3A7F6E}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>